<commit_message>
Updated layout from journal
</commit_message>
<xml_diff>
--- a/management/dagboek.xlsx
+++ b/management/dagboek.xlsx
@@ -111,16 +111,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -401,127 +417,135 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="6">
         <f ca="1">TODAY()</f>
         <v>42780</v>
       </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="6">
         <v>42688</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="6">
         <v>42689</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="10" t="s">
         <v>8</v>
       </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="6">
         <v>42690</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="10" t="s">
         <v>8</v>
       </c>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="6">
         <v>42691</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="10" t="s">
         <v>8</v>
       </c>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="6">
         <v>42692</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="10" t="s">
         <v>8</v>
       </c>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="6">
         <v>42701</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="10" t="s">
         <v>8</v>
       </c>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="6">
         <v>42780</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="10" t="s">
         <v>11</v>
       </c>
+      <c r="D10" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added todays entry in journal
</commit_message>
<xml_diff>
--- a/management/dagboek.xlsx
+++ b/management/dagboek.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>DAGBOEK PROJECTWERK</t>
   </si>
@@ -32,9 +32,6 @@
     <t>AUTHORS:</t>
   </si>
   <si>
-    <t>PIETER DELOBELLE, ANTON DANNEELS, MATTHIAS DE LANGHE</t>
-  </si>
-  <si>
     <t>UPDATE:</t>
   </si>
   <si>
@@ -60,6 +57,12 @@
   </si>
   <si>
     <t>ON TRACK</t>
+  </si>
+  <si>
+    <t>Persistence context configureren</t>
+  </si>
+  <si>
+    <t>PIETER DELOBELLE, ANTON DANNEELS, MATTHIAS DE LANGE</t>
   </si>
 </sst>
 </file>
@@ -125,17 +128,17 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,51 +430,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
-        <v>3</v>
       </c>
       <c r="D2" s="6">
         <f ca="1">TODAY()</f>
-        <v>42780</v>
+        <v>42786</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>42688</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -480,10 +483,10 @@
         <v>42689</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -492,10 +495,10 @@
         <v>42690</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -504,10 +507,10 @@
         <v>42691</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D7" s="4"/>
     </row>
@@ -516,10 +519,10 @@
         <v>42692</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -528,10 +531,10 @@
         <v>42701</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="10" t="s">
         <v>8</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D9" s="4"/>
     </row>
@@ -540,12 +543,23 @@
         <v>42780</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>42786</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>